<commit_message>
2023/05/26 British 페르소나 데이터 수정
</commit_message>
<xml_diff>
--- a/src/data/British.xlsx
+++ b/src/data/British.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\윤덕건\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\윤덕건\Desktop\1줄 설명\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA2EBF1-BC1F-4C26-B141-845C34D204A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C920D3-1AFF-4EF6-A5A3-8A9DBAADB313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6692" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6692" uniqueCount="520">
   <si>
     <t>user</t>
   </si>
@@ -1577,6 +1577,10 @@
   </si>
   <si>
     <t>힐튼 메이페어 카지노(Hilton Metropole Casino)는 런던의 웨스트미니스터(Westminster) 지역에 위치한 카지노입니다. 이 카지노는 힐튼 호텔과 연계되어 있으며, 다양한 도박 게임과 슬롯 머신을 제공합니다. 카지노 내부에는 현대적이고 우아한 분위기가 조성되어 있으며, 고급스러운 레스토랑과 바도 함께 운영되고 있습니다. 힐튼 메이페어 카지노는 카지노 게임을 즐기고자 하는 방문객들에게 편안하고 멋진 경험을 제공합니다.</t>
+  </si>
+  <si>
+    <t>술과 음식</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1650,7 +1654,648 @@
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="64">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1950,8 +2595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1672"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A1596" workbookViewId="0">
+      <selection activeCell="O1622" sqref="O1622"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -2166,7 +2811,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
         <v>30</v>
@@ -2192,7 +2837,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
         <v>33</v>
@@ -2218,7 +2863,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
         <v>36</v>
@@ -2244,7 +2889,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
         <v>39</v>
@@ -2400,7 +3045,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s">
         <v>57</v>
@@ -2426,7 +3071,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B19" t="s">
         <v>60</v>
@@ -5009,7 +5654,7 @@
         <v>3</v>
       </c>
       <c r="D118" t="s">
-        <v>291</v>
+        <v>519</v>
       </c>
       <c r="E118">
         <v>53.402035012823497</v>
@@ -6745,25 +7390,25 @@
         <v>53</v>
       </c>
       <c r="B185" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C185">
         <v>4</v>
       </c>
       <c r="D185" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E185">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F185">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G185" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H185" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.45">
@@ -9397,25 +10042,25 @@
         <v>60</v>
       </c>
       <c r="B287" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C287">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D287" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E287">
-        <v>51.513047933947199</v>
+        <v>51.505609966881202</v>
       </c>
       <c r="F287">
-        <v>-0.122133229092797</v>
+        <v>-7.5206298403609498E-2</v>
       </c>
       <c r="G287" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H287" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="288" spans="1:8" x14ac:dyDescent="0.45">
@@ -9449,25 +10094,25 @@
         <v>61</v>
       </c>
       <c r="B289" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C289">
         <v>4</v>
       </c>
       <c r="D289" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E289">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F289">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G289" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H289" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="290" spans="1:8" x14ac:dyDescent="0.45">
@@ -9527,25 +10172,25 @@
         <v>61</v>
       </c>
       <c r="B292" t="s">
-        <v>21</v>
+        <v>205</v>
       </c>
       <c r="C292">
         <v>4</v>
       </c>
       <c r="D292" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E292">
-        <v>51.5077488596718</v>
+        <v>51.503427939108001</v>
       </c>
       <c r="F292">
-        <v>-9.92920290930428E-2</v>
+        <v>-0.119170113194877</v>
       </c>
       <c r="G292" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
       <c r="H292" t="s">
-        <v>23</v>
+        <v>208</v>
       </c>
     </row>
     <row r="293" spans="1:8" x14ac:dyDescent="0.45">
@@ -9683,25 +10328,25 @@
         <v>61</v>
       </c>
       <c r="B298" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C298">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D298" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E298">
-        <v>51.513047933947199</v>
+        <v>51.505609966881202</v>
       </c>
       <c r="F298">
-        <v>-0.122133229092797</v>
+        <v>-7.5206298403609498E-2</v>
       </c>
       <c r="G298" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H298" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="299" spans="1:8" x14ac:dyDescent="0.45">
@@ -10203,25 +10848,25 @@
         <v>64</v>
       </c>
       <c r="B318" t="s">
-        <v>21</v>
+        <v>205</v>
       </c>
       <c r="C318">
         <v>4</v>
       </c>
       <c r="D318" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E318">
-        <v>51.5077488596718</v>
+        <v>51.503427939108001</v>
       </c>
       <c r="F318">
-        <v>-9.92920290930428E-2</v>
+        <v>-0.119170113194877</v>
       </c>
       <c r="G318" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
       <c r="H318" t="s">
-        <v>23</v>
+        <v>208</v>
       </c>
     </row>
     <row r="319" spans="1:8" x14ac:dyDescent="0.45">
@@ -10463,25 +11108,25 @@
         <v>65</v>
       </c>
       <c r="B328" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C328">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D328" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E328">
-        <v>51.513047933947199</v>
+        <v>51.505609966881202</v>
       </c>
       <c r="F328">
-        <v>-0.122133229092797</v>
+        <v>-7.5206298403609498E-2</v>
       </c>
       <c r="G328" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H328" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="329" spans="1:8" x14ac:dyDescent="0.45">
@@ -10775,25 +11420,25 @@
         <v>65</v>
       </c>
       <c r="B340" t="s">
-        <v>21</v>
+        <v>205</v>
       </c>
       <c r="C340">
         <v>4</v>
       </c>
       <c r="D340" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E340">
-        <v>51.5077488596718</v>
+        <v>51.503427939108001</v>
       </c>
       <c r="F340">
-        <v>-9.92920290930428E-2</v>
+        <v>-0.119170113194877</v>
       </c>
       <c r="G340" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
       <c r="H340" t="s">
-        <v>23</v>
+        <v>208</v>
       </c>
     </row>
     <row r="341" spans="1:8" x14ac:dyDescent="0.45">
@@ -11113,25 +11758,25 @@
         <v>67</v>
       </c>
       <c r="B353" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C353">
         <v>4</v>
       </c>
       <c r="D353" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E353">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F353">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G353" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H353" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="354" spans="1:8" x14ac:dyDescent="0.45">
@@ -11191,25 +11836,25 @@
         <v>67</v>
       </c>
       <c r="B356" t="s">
-        <v>21</v>
+        <v>205</v>
       </c>
       <c r="C356">
         <v>4</v>
       </c>
       <c r="D356" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E356">
-        <v>51.5077488596718</v>
+        <v>51.503427939108001</v>
       </c>
       <c r="F356">
-        <v>-9.92920290930428E-2</v>
+        <v>-0.119170113194877</v>
       </c>
       <c r="G356" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
       <c r="H356" t="s">
-        <v>23</v>
+        <v>208</v>
       </c>
     </row>
     <row r="357" spans="1:8" x14ac:dyDescent="0.45">
@@ -12985,25 +13630,25 @@
         <v>73</v>
       </c>
       <c r="B425" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C425">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D425" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E425">
-        <v>51.513047933947199</v>
+        <v>51.505609966881202</v>
       </c>
       <c r="F425">
-        <v>-0.122133229092797</v>
+        <v>-7.5206298403609498E-2</v>
       </c>
       <c r="G425" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H425" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="426" spans="1:8" x14ac:dyDescent="0.45">
@@ -13011,25 +13656,25 @@
         <v>73</v>
       </c>
       <c r="B426" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C426">
         <v>4</v>
       </c>
       <c r="D426" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E426">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F426">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G426" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H426" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="427" spans="1:8" x14ac:dyDescent="0.45">
@@ -14389,25 +15034,25 @@
         <v>79</v>
       </c>
       <c r="B479" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C479">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D479" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E479">
-        <v>51.513047933947199</v>
+        <v>51.505609966881202</v>
       </c>
       <c r="F479">
-        <v>-0.122133229092797</v>
+        <v>-7.5206298403609498E-2</v>
       </c>
       <c r="G479" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H479" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="480" spans="1:8" x14ac:dyDescent="0.45">
@@ -17431,25 +18076,25 @@
         <v>90</v>
       </c>
       <c r="B596" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C596">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D596" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E596">
-        <v>51.513047933947199</v>
+        <v>51.505609966881202</v>
       </c>
       <c r="F596">
-        <v>-0.122133229092797</v>
+        <v>-7.5206298403609498E-2</v>
       </c>
       <c r="G596" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H596" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="597" spans="1:8" x14ac:dyDescent="0.45">
@@ -17769,25 +18414,25 @@
         <v>91</v>
       </c>
       <c r="B609" t="s">
-        <v>21</v>
+        <v>205</v>
       </c>
       <c r="C609">
         <v>4</v>
       </c>
       <c r="D609" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E609">
-        <v>51.5077488596718</v>
+        <v>51.503427939108001</v>
       </c>
       <c r="F609">
-        <v>-9.92920290930428E-2</v>
+        <v>-0.119170113194877</v>
       </c>
       <c r="G609" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
       <c r="H609" t="s">
-        <v>23</v>
+        <v>208</v>
       </c>
     </row>
     <row r="610" spans="1:8" x14ac:dyDescent="0.45">
@@ -18783,25 +19428,25 @@
         <v>94</v>
       </c>
       <c r="B648" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C648">
         <v>4</v>
       </c>
       <c r="D648" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E648">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F648">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G648" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H648" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="649" spans="1:8" x14ac:dyDescent="0.45">
@@ -19225,25 +19870,25 @@
         <v>95</v>
       </c>
       <c r="B665" t="s">
-        <v>21</v>
+        <v>205</v>
       </c>
       <c r="C665">
         <v>4</v>
       </c>
       <c r="D665" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E665">
-        <v>51.5077488596718</v>
+        <v>51.503427939108001</v>
       </c>
       <c r="F665">
-        <v>-9.92920290930428E-2</v>
+        <v>-0.119170113194877</v>
       </c>
       <c r="G665" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
       <c r="H665" t="s">
-        <v>23</v>
+        <v>208</v>
       </c>
     </row>
     <row r="666" spans="1:8" x14ac:dyDescent="0.45">
@@ -19589,25 +20234,25 @@
         <v>96</v>
       </c>
       <c r="B679" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C679">
         <v>4</v>
       </c>
       <c r="D679" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E679">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F679">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G679" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H679" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="680" spans="1:8" x14ac:dyDescent="0.45">
@@ -19667,25 +20312,25 @@
         <v>96</v>
       </c>
       <c r="B682" t="s">
-        <v>21</v>
+        <v>205</v>
       </c>
       <c r="C682">
         <v>4</v>
       </c>
       <c r="D682" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E682">
-        <v>51.5077488596718</v>
+        <v>51.503427939108001</v>
       </c>
       <c r="F682">
-        <v>-9.92920290930428E-2</v>
+        <v>-0.119170113194877</v>
       </c>
       <c r="G682" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
       <c r="H682" t="s">
-        <v>23</v>
+        <v>208</v>
       </c>
     </row>
     <row r="683" spans="1:8" x14ac:dyDescent="0.45">
@@ -19979,25 +20624,25 @@
         <v>96</v>
       </c>
       <c r="B694" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C694">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D694" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E694">
-        <v>51.513047933947199</v>
+        <v>51.505609966881202</v>
       </c>
       <c r="F694">
-        <v>-0.122133229092797</v>
+        <v>-7.5206298403609498E-2</v>
       </c>
       <c r="G694" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H694" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="695" spans="1:8" x14ac:dyDescent="0.45">
@@ -20993,25 +21638,25 @@
         <v>99</v>
       </c>
       <c r="B733" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C733">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D733" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E733">
-        <v>51.513047933947199</v>
+        <v>51.505609966881202</v>
       </c>
       <c r="F733">
-        <v>-0.122133229092797</v>
+        <v>-7.5206298403609498E-2</v>
       </c>
       <c r="G733" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H733" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="734" spans="1:8" x14ac:dyDescent="0.45">
@@ -21019,25 +21664,25 @@
         <v>99</v>
       </c>
       <c r="B734" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C734">
         <v>4</v>
       </c>
       <c r="D734" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E734">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F734">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G734" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H734" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="735" spans="1:8" x14ac:dyDescent="0.45">
@@ -21409,25 +22054,25 @@
         <v>100</v>
       </c>
       <c r="B749" t="s">
-        <v>21</v>
+        <v>205</v>
       </c>
       <c r="C749">
         <v>4</v>
       </c>
       <c r="D749" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E749">
-        <v>51.5077488596718</v>
+        <v>51.503427939108001</v>
       </c>
       <c r="F749">
-        <v>-9.92920290930428E-2</v>
+        <v>-0.119170113194877</v>
       </c>
       <c r="G749" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
       <c r="H749" t="s">
-        <v>23</v>
+        <v>208</v>
       </c>
     </row>
     <row r="750" spans="1:8" x14ac:dyDescent="0.45">
@@ -21877,25 +22522,25 @@
         <v>102</v>
       </c>
       <c r="B767" t="s">
-        <v>21</v>
+        <v>205</v>
       </c>
       <c r="C767">
         <v>4</v>
       </c>
       <c r="D767" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E767">
-        <v>51.5077488596718</v>
+        <v>51.503427939108001</v>
       </c>
       <c r="F767">
-        <v>-9.92920290930428E-2</v>
+        <v>-0.119170113194877</v>
       </c>
       <c r="G767" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
       <c r="H767" t="s">
-        <v>23</v>
+        <v>208</v>
       </c>
     </row>
     <row r="768" spans="1:8" x14ac:dyDescent="0.45">
@@ -23047,25 +23692,25 @@
         <v>105</v>
       </c>
       <c r="B812" t="s">
-        <v>21</v>
+        <v>205</v>
       </c>
       <c r="C812">
         <v>4</v>
       </c>
       <c r="D812" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E812">
-        <v>51.5077488596718</v>
+        <v>51.503427939108001</v>
       </c>
       <c r="F812">
-        <v>-9.92920290930428E-2</v>
+        <v>-0.119170113194877</v>
       </c>
       <c r="G812" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
       <c r="H812" t="s">
-        <v>23</v>
+        <v>208</v>
       </c>
     </row>
     <row r="813" spans="1:8" x14ac:dyDescent="0.45">
@@ -23801,25 +24446,25 @@
         <v>107</v>
       </c>
       <c r="B841" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C841">
         <v>4</v>
       </c>
       <c r="D841" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E841">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F841">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G841" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H841" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="842" spans="1:8" x14ac:dyDescent="0.45">
@@ -23879,25 +24524,25 @@
         <v>107</v>
       </c>
       <c r="B844" t="s">
-        <v>21</v>
+        <v>205</v>
       </c>
       <c r="C844">
         <v>4</v>
       </c>
       <c r="D844" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E844">
-        <v>51.5077488596718</v>
+        <v>51.503427939108001</v>
       </c>
       <c r="F844">
-        <v>-9.92920290930428E-2</v>
+        <v>-0.119170113194877</v>
       </c>
       <c r="G844" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
       <c r="H844" t="s">
-        <v>23</v>
+        <v>208</v>
       </c>
     </row>
     <row r="845" spans="1:8" x14ac:dyDescent="0.45">
@@ -24321,25 +24966,25 @@
         <v>108</v>
       </c>
       <c r="B861" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C861">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D861" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E861">
-        <v>51.513047933947199</v>
+        <v>51.505609966881202</v>
       </c>
       <c r="F861">
-        <v>-0.122133229092797</v>
+        <v>-7.5206298403609498E-2</v>
       </c>
       <c r="G861" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H861" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="862" spans="1:8" x14ac:dyDescent="0.45">
@@ -24659,25 +25304,25 @@
         <v>108</v>
       </c>
       <c r="B874" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C874">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D874" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E874">
-        <v>51.513047933947199</v>
+        <v>51.505609966881202</v>
       </c>
       <c r="F874">
-        <v>-0.122133229092797</v>
+        <v>-7.5206298403609498E-2</v>
       </c>
       <c r="G874" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H874" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="875" spans="1:8" x14ac:dyDescent="0.45">
@@ -25049,25 +25694,25 @@
         <v>109</v>
       </c>
       <c r="B889" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C889">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D889" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E889">
-        <v>51.513047933947199</v>
+        <v>51.505609966881202</v>
       </c>
       <c r="F889">
-        <v>-0.122133229092797</v>
+        <v>-7.5206298403609498E-2</v>
       </c>
       <c r="G889" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H889" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="890" spans="1:8" x14ac:dyDescent="0.45">
@@ -25465,25 +26110,25 @@
         <v>111</v>
       </c>
       <c r="B905" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C905">
         <v>4</v>
       </c>
       <c r="D905" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E905">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F905">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G905" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H905" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="906" spans="1:8" x14ac:dyDescent="0.45">
@@ -25855,25 +26500,25 @@
         <v>111</v>
       </c>
       <c r="B920" t="s">
-        <v>21</v>
+        <v>205</v>
       </c>
       <c r="C920">
         <v>4</v>
       </c>
       <c r="D920" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E920">
-        <v>51.5077488596718</v>
+        <v>51.503427939108001</v>
       </c>
       <c r="F920">
-        <v>-9.92920290930428E-2</v>
+        <v>-0.119170113194877</v>
       </c>
       <c r="G920" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
       <c r="H920" t="s">
-        <v>23</v>
+        <v>208</v>
       </c>
     </row>
     <row r="921" spans="1:8" x14ac:dyDescent="0.45">
@@ -26739,25 +27384,25 @@
         <v>114</v>
       </c>
       <c r="B954" t="s">
-        <v>21</v>
+        <v>205</v>
       </c>
       <c r="C954">
         <v>4</v>
       </c>
       <c r="D954" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E954">
-        <v>51.5077488596718</v>
+        <v>51.503427939108001</v>
       </c>
       <c r="F954">
-        <v>-9.92920290930428E-2</v>
+        <v>-0.119170113194877</v>
       </c>
       <c r="G954" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
       <c r="H954" t="s">
-        <v>23</v>
+        <v>208</v>
       </c>
     </row>
     <row r="955" spans="1:8" x14ac:dyDescent="0.45">
@@ -28091,25 +28736,25 @@
         <v>117</v>
       </c>
       <c r="B1006" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C1006">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1006" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1006">
-        <v>51.513047933947199</v>
+        <v>51.505609966881202</v>
       </c>
       <c r="F1006">
-        <v>-0.122133229092797</v>
+        <v>-7.5206298403609498E-2</v>
       </c>
       <c r="G1006" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H1006" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1007" spans="1:8" x14ac:dyDescent="0.45">
@@ -28429,25 +29074,25 @@
         <v>118</v>
       </c>
       <c r="B1019" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C1019">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1019" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1019">
-        <v>51.513047933947199</v>
+        <v>51.505609966881202</v>
       </c>
       <c r="F1019">
-        <v>-0.122133229092797</v>
+        <v>-7.5206298403609498E-2</v>
       </c>
       <c r="G1019" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H1019" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1020" spans="1:8" x14ac:dyDescent="0.45">
@@ -28793,25 +29438,25 @@
         <v>119</v>
       </c>
       <c r="B1033" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C1033">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1033" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1033">
-        <v>51.513047933947199</v>
+        <v>51.505609966881202</v>
       </c>
       <c r="F1033">
-        <v>-0.122133229092797</v>
+        <v>-7.5206298403609498E-2</v>
       </c>
       <c r="G1033" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H1033" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1034" spans="1:8" x14ac:dyDescent="0.45">
@@ -29131,25 +29776,25 @@
         <v>120</v>
       </c>
       <c r="B1046" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C1046">
         <v>4</v>
       </c>
       <c r="D1046" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1046">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F1046">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G1046" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H1046" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="1047" spans="1:8" x14ac:dyDescent="0.45">
@@ -29469,25 +30114,25 @@
         <v>121</v>
       </c>
       <c r="B1059" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C1059">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1059" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1059">
-        <v>51.513047933947199</v>
+        <v>51.505609966881202</v>
       </c>
       <c r="F1059">
-        <v>-0.122133229092797</v>
+        <v>-7.5206298403609498E-2</v>
       </c>
       <c r="G1059" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H1059" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1060" spans="1:8" x14ac:dyDescent="0.45">
@@ -29729,25 +30374,25 @@
         <v>122</v>
       </c>
       <c r="B1069" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C1069">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1069" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1069">
-        <v>51.513047933947199</v>
+        <v>51.505609966881202</v>
       </c>
       <c r="F1069">
-        <v>-0.122133229092797</v>
+        <v>-7.5206298403609498E-2</v>
       </c>
       <c r="G1069" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H1069" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1070" spans="1:8" x14ac:dyDescent="0.45">
@@ -31185,25 +31830,25 @@
         <v>126</v>
       </c>
       <c r="B1125" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C1125">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1125" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1125">
-        <v>51.513047933947199</v>
+        <v>51.505609966881202</v>
       </c>
       <c r="F1125">
-        <v>-0.122133229092797</v>
+        <v>-7.5206298403609498E-2</v>
       </c>
       <c r="G1125" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H1125" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1126" spans="1:8" x14ac:dyDescent="0.45">
@@ -31913,25 +32558,25 @@
         <v>128</v>
       </c>
       <c r="B1153" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C1153">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1153" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1153">
-        <v>51.513047933947199</v>
+        <v>51.505609966881202</v>
       </c>
       <c r="F1153">
-        <v>-0.122133229092797</v>
+        <v>-7.5206298403609498E-2</v>
       </c>
       <c r="G1153" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H1153" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1154" spans="1:8" x14ac:dyDescent="0.45">
@@ -32199,25 +32844,25 @@
         <v>129</v>
       </c>
       <c r="B1164" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C1164">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1164" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1164">
-        <v>51.513047933947199</v>
+        <v>51.505609966881202</v>
       </c>
       <c r="F1164">
-        <v>-0.122133229092797</v>
+        <v>-7.5206298403609498E-2</v>
       </c>
       <c r="G1164" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H1164" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1165" spans="1:8" x14ac:dyDescent="0.45">
@@ -32225,25 +32870,25 @@
         <v>129</v>
       </c>
       <c r="B1165" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C1165">
         <v>4</v>
       </c>
       <c r="D1165" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1165">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F1165">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G1165" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H1165" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="1166" spans="1:8" x14ac:dyDescent="0.45">
@@ -32641,25 +33286,25 @@
         <v>130</v>
       </c>
       <c r="B1181" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C1181">
         <v>4</v>
       </c>
       <c r="D1181" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1181">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F1181">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G1181" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H1181" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="1182" spans="1:8" x14ac:dyDescent="0.45">
@@ -33031,25 +33676,25 @@
         <v>131</v>
       </c>
       <c r="B1196" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C1196">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1196" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1196">
-        <v>51.513047933947199</v>
+        <v>51.505609966881202</v>
       </c>
       <c r="F1196">
-        <v>-0.122133229092797</v>
+        <v>-7.5206298403609498E-2</v>
       </c>
       <c r="G1196" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H1196" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1197" spans="1:8" x14ac:dyDescent="0.45">
@@ -33551,25 +34196,25 @@
         <v>133</v>
       </c>
       <c r="B1216" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C1216">
         <v>4</v>
       </c>
       <c r="D1216" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1216">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F1216">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G1216" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H1216" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="1217" spans="1:8" x14ac:dyDescent="0.45">
@@ -33967,25 +34612,25 @@
         <v>134</v>
       </c>
       <c r="B1232" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C1232">
         <v>4</v>
       </c>
       <c r="D1232" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1232">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F1232">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G1232" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H1232" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="1233" spans="1:8" x14ac:dyDescent="0.45">
@@ -34175,25 +34820,25 @@
         <v>135</v>
       </c>
       <c r="B1240" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C1240">
         <v>4</v>
       </c>
       <c r="D1240" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1240">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F1240">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G1240" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H1240" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="1241" spans="1:8" x14ac:dyDescent="0.45">
@@ -34383,25 +35028,25 @@
         <v>136</v>
       </c>
       <c r="B1248" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C1248">
         <v>4</v>
       </c>
       <c r="D1248" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1248">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F1248">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G1248" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H1248" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="1249" spans="1:8" x14ac:dyDescent="0.45">
@@ -34955,25 +35600,25 @@
         <v>138</v>
       </c>
       <c r="B1270" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C1270">
         <v>4</v>
       </c>
       <c r="D1270" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1270">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F1270">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G1270" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H1270" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="1271" spans="1:8" x14ac:dyDescent="0.45">
@@ -35709,25 +36354,25 @@
         <v>141</v>
       </c>
       <c r="B1299" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C1299">
         <v>4</v>
       </c>
       <c r="D1299" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1299">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F1299">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G1299" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H1299" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="1300" spans="1:8" x14ac:dyDescent="0.45">
@@ -37269,25 +37914,25 @@
         <v>147</v>
       </c>
       <c r="B1359" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C1359">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1359" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1359">
-        <v>51.513047933947199</v>
+        <v>51.505609966881202</v>
       </c>
       <c r="F1359">
-        <v>-0.122133229092797</v>
+        <v>-7.5206298403609498E-2</v>
       </c>
       <c r="G1359" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H1359" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1360" spans="1:8" x14ac:dyDescent="0.45">
@@ -37295,25 +37940,25 @@
         <v>147</v>
       </c>
       <c r="B1360" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C1360">
         <v>4</v>
       </c>
       <c r="D1360" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1360">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F1360">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G1360" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H1360" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="1361" spans="1:8" x14ac:dyDescent="0.45">
@@ -37971,25 +38616,25 @@
         <v>150</v>
       </c>
       <c r="B1386" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C1386">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1386" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1386">
-        <v>51.513047933947199</v>
+        <v>51.505609966881202</v>
       </c>
       <c r="F1386">
-        <v>-0.122133229092797</v>
+        <v>-7.5206298403609498E-2</v>
       </c>
       <c r="G1386" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H1386" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1387" spans="1:8" x14ac:dyDescent="0.45">
@@ -38413,25 +39058,25 @@
         <v>152</v>
       </c>
       <c r="B1403" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C1403">
         <v>4</v>
       </c>
       <c r="D1403" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1403">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F1403">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G1403" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H1403" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="1404" spans="1:8" x14ac:dyDescent="0.45">
@@ -38803,25 +39448,25 @@
         <v>153</v>
       </c>
       <c r="B1418" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C1418">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1418" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1418">
-        <v>51.513047933947199</v>
+        <v>51.505609966881202</v>
       </c>
       <c r="F1418">
-        <v>-0.122133229092797</v>
+        <v>-7.5206298403609498E-2</v>
       </c>
       <c r="G1418" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H1418" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1419" spans="1:8" x14ac:dyDescent="0.45">
@@ -38829,25 +39474,25 @@
         <v>153</v>
       </c>
       <c r="B1419" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C1419">
         <v>4</v>
       </c>
       <c r="D1419" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1419">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F1419">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G1419" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H1419" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="1420" spans="1:8" x14ac:dyDescent="0.45">
@@ -39141,25 +39786,25 @@
         <v>154</v>
       </c>
       <c r="B1431" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C1431">
         <v>4</v>
       </c>
       <c r="D1431" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1431">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F1431">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G1431" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H1431" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="1432" spans="1:8" x14ac:dyDescent="0.45">
@@ -40493,25 +41138,25 @@
         <v>159</v>
       </c>
       <c r="B1483" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C1483">
         <v>4</v>
       </c>
       <c r="D1483" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1483">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F1483">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G1483" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H1483" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="1484" spans="1:8" x14ac:dyDescent="0.45">
@@ -40727,25 +41372,25 @@
         <v>160</v>
       </c>
       <c r="B1492" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C1492">
         <v>4</v>
       </c>
       <c r="D1492" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1492">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F1492">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G1492" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H1492" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="1493" spans="1:8" x14ac:dyDescent="0.45">
@@ -41039,25 +41684,25 @@
         <v>161</v>
       </c>
       <c r="B1504" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C1504">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1504" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1504">
-        <v>51.513047933947199</v>
+        <v>51.505609966881202</v>
       </c>
       <c r="F1504">
-        <v>-0.122133229092797</v>
+        <v>-7.5206298403609498E-2</v>
       </c>
       <c r="G1504" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H1504" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1505" spans="1:8" x14ac:dyDescent="0.45">
@@ -41065,25 +41710,25 @@
         <v>161</v>
       </c>
       <c r="B1505" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C1505">
         <v>4</v>
       </c>
       <c r="D1505" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1505">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F1505">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G1505" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H1505" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="1506" spans="1:8" x14ac:dyDescent="0.45">
@@ -41689,25 +42334,25 @@
         <v>163</v>
       </c>
       <c r="B1529" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C1529">
         <v>4</v>
       </c>
       <c r="D1529" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1529">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F1529">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G1529" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H1529" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="1530" spans="1:8" x14ac:dyDescent="0.45">
@@ -43041,25 +43686,25 @@
         <v>167</v>
       </c>
       <c r="B1581" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C1581">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1581" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1581">
-        <v>51.513047933947199</v>
+        <v>51.505609966881202</v>
       </c>
       <c r="F1581">
-        <v>-0.122133229092797</v>
+        <v>-7.5206298403609498E-2</v>
       </c>
       <c r="G1581" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H1581" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1582" spans="1:8" x14ac:dyDescent="0.45">
@@ -43067,25 +43712,25 @@
         <v>167</v>
       </c>
       <c r="B1582" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C1582">
         <v>4</v>
       </c>
       <c r="D1582" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1582">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F1582">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G1582" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H1582" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="1583" spans="1:8" x14ac:dyDescent="0.45">
@@ -43353,25 +43998,25 @@
         <v>168</v>
       </c>
       <c r="B1593" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C1593">
         <v>4</v>
       </c>
       <c r="D1593" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1593">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F1593">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G1593" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H1593" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="1594" spans="1:8" x14ac:dyDescent="0.45">
@@ -43665,25 +44310,25 @@
         <v>169</v>
       </c>
       <c r="B1605" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C1605">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1605" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1605">
-        <v>51.513047933947199</v>
+        <v>51.505609966881202</v>
       </c>
       <c r="F1605">
-        <v>-0.122133229092797</v>
+        <v>-7.5206298403609498E-2</v>
       </c>
       <c r="G1605" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H1605" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1606" spans="1:8" x14ac:dyDescent="0.45">
@@ -43951,25 +44596,25 @@
         <v>170</v>
       </c>
       <c r="B1616" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C1616">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1616" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1616">
-        <v>51.513047933947199</v>
+        <v>51.505609966881202</v>
       </c>
       <c r="F1616">
-        <v>-0.122133229092797</v>
+        <v>-7.5206298403609498E-2</v>
       </c>
       <c r="G1616" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H1616" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1617" spans="1:8" x14ac:dyDescent="0.45">
@@ -44289,25 +44934,25 @@
         <v>171</v>
       </c>
       <c r="B1629" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C1629">
         <v>4</v>
       </c>
       <c r="D1629" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1629">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F1629">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G1629" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H1629" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="1630" spans="1:8" x14ac:dyDescent="0.45">
@@ -44679,25 +45324,25 @@
         <v>172</v>
       </c>
       <c r="B1644" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C1644">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1644" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1644">
-        <v>51.513047933947199</v>
+        <v>51.505609966881202</v>
       </c>
       <c r="F1644">
-        <v>-0.122133229092797</v>
+        <v>-7.5206298403609498E-2</v>
       </c>
       <c r="G1644" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H1644" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="1645" spans="1:8" x14ac:dyDescent="0.45">
@@ -45017,25 +45662,25 @@
         <v>173</v>
       </c>
       <c r="B1657" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C1657">
         <v>4</v>
       </c>
       <c r="D1657" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1657">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F1657">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G1657" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H1657" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="1658" spans="1:8" x14ac:dyDescent="0.45">
@@ -45329,25 +45974,25 @@
         <v>174</v>
       </c>
       <c r="B1669" t="s">
-        <v>12</v>
+        <v>451</v>
       </c>
       <c r="C1669">
         <v>4</v>
       </c>
       <c r="D1669" t="s">
-        <v>9</v>
+        <v>452</v>
       </c>
       <c r="E1669">
-        <v>51.496846231186097</v>
+        <v>51.500802638007897</v>
       </c>
       <c r="F1669">
-        <v>-0.17182595051629301</v>
+        <v>-0.12430353779023701</v>
       </c>
       <c r="G1669" t="s">
-        <v>13</v>
+        <v>453</v>
       </c>
       <c r="H1669" t="s">
-        <v>14</v>
+        <v>454</v>
       </c>
     </row>
     <row r="1670" spans="1:8" x14ac:dyDescent="0.45">
@@ -45430,6 +46075,192 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="B185">
+    <cfRule type="duplicateValues" dxfId="63" priority="62"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B185">
+    <cfRule type="duplicateValues" dxfId="62" priority="61"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B289">
+    <cfRule type="duplicateValues" dxfId="61" priority="60"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B289">
+    <cfRule type="duplicateValues" dxfId="60" priority="59"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B353">
+    <cfRule type="duplicateValues" dxfId="59" priority="58"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B353">
+    <cfRule type="duplicateValues" dxfId="58" priority="57"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B426">
+    <cfRule type="duplicateValues" dxfId="57" priority="56"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B426">
+    <cfRule type="duplicateValues" dxfId="56" priority="55"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B648">
+    <cfRule type="duplicateValues" dxfId="55" priority="54"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B648">
+    <cfRule type="duplicateValues" dxfId="54" priority="53"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B679">
+    <cfRule type="duplicateValues" dxfId="53" priority="52"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B679">
+    <cfRule type="duplicateValues" dxfId="52" priority="51"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B734">
+    <cfRule type="duplicateValues" dxfId="51" priority="50"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B734">
+    <cfRule type="duplicateValues" dxfId="50" priority="49"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B841">
+    <cfRule type="duplicateValues" dxfId="49" priority="48"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B841">
+    <cfRule type="duplicateValues" dxfId="48" priority="47"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1216">
+    <cfRule type="duplicateValues" dxfId="47" priority="46"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1216">
+    <cfRule type="duplicateValues" dxfId="46" priority="45"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1232">
+    <cfRule type="duplicateValues" dxfId="43" priority="44"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1232">
+    <cfRule type="duplicateValues" dxfId="42" priority="43"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1360">
+    <cfRule type="duplicateValues" dxfId="41" priority="42"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1360">
+    <cfRule type="duplicateValues" dxfId="40" priority="41"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1419">
+    <cfRule type="duplicateValues" dxfId="39" priority="40"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1419">
+    <cfRule type="duplicateValues" dxfId="38" priority="39"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1492">
+    <cfRule type="duplicateValues" dxfId="37" priority="38"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1492">
+    <cfRule type="duplicateValues" dxfId="36" priority="37"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1629">
+    <cfRule type="duplicateValues" dxfId="35" priority="36"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1629">
+    <cfRule type="duplicateValues" dxfId="34" priority="35"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1669">
+    <cfRule type="duplicateValues" dxfId="33" priority="34"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1669">
+    <cfRule type="duplicateValues" dxfId="32" priority="33"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1657">
+    <cfRule type="duplicateValues" dxfId="31" priority="32"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1657">
+    <cfRule type="duplicateValues" dxfId="30" priority="31"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1582">
+    <cfRule type="duplicateValues" dxfId="29" priority="30"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1582">
+    <cfRule type="duplicateValues" dxfId="28" priority="29"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1529">
+    <cfRule type="duplicateValues" dxfId="27" priority="28"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1529">
+    <cfRule type="duplicateValues" dxfId="26" priority="27"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1483">
+    <cfRule type="duplicateValues" dxfId="25" priority="26"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1483">
+    <cfRule type="duplicateValues" dxfId="24" priority="25"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1403">
+    <cfRule type="duplicateValues" dxfId="23" priority="24"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1403">
+    <cfRule type="duplicateValues" dxfId="22" priority="23"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1240">
+    <cfRule type="duplicateValues" dxfId="21" priority="22"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1240">
+    <cfRule type="duplicateValues" dxfId="20" priority="21"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B905">
+    <cfRule type="duplicateValues" dxfId="19" priority="20"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B905">
+    <cfRule type="duplicateValues" dxfId="18" priority="19"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1046">
+    <cfRule type="duplicateValues" dxfId="17" priority="18"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1046">
+    <cfRule type="duplicateValues" dxfId="16" priority="17"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1165">
+    <cfRule type="duplicateValues" dxfId="15" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1165">
+    <cfRule type="duplicateValues" dxfId="14" priority="15"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1270">
+    <cfRule type="duplicateValues" dxfId="13" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1270">
+    <cfRule type="duplicateValues" dxfId="12" priority="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1431">
+    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1431">
+    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1505">
+    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1505">
+    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1593">
+    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1593">
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1248">
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1248">
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1181">
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1181">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1299">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1299">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>